<commit_message>
next try, the readin used to skip ra rows, but now it does not
</commit_message>
<xml_diff>
--- a/tests/data/results_0012_combined.xlsx
+++ b/tests/data/results_0012_combined.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dtudk-my.sharepoint.com/personal/mittma_dtu_dk/Documents/Dokumenter/Programming/practices/EDX code/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mittma\AppData\Local\Packages\CanonicalGroupLimited.Ubuntu_79rhkp1fndgsc\LocalState\rootfs\home\mittma\nomad-dtu-nanolab-plugin\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="25" documentId="8_{F25A7F45-DEBC-46F6-B1FD-EB25EE3FB7D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C0055DB9-A00A-42CD-9FEA-873D387FD977}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE091B38-E3F5-4B72-9E07-B8C018E47FFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
   <si>
     <t>Spectrum Label</t>
   </si>
@@ -153,9 +153,6 @@
   </si>
   <si>
     <t>FL 15</t>
-  </si>
-  <si>
-    <t>middle</t>
   </si>
   <si>
     <t>BR1</t>
@@ -305,10 +302,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -574,10 +567,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J62"/>
+  <dimension ref="A1:J61"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="J33" sqref="J33"/>
+      <selection activeCell="Q41" sqref="Q41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -611,7 +604,7 @@
         <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
@@ -676,7 +669,7 @@
         <v>38.49</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J62" si="0">G3/H3</f>
+        <f t="shared" ref="J3:J61" si="0">G3/H3</f>
         <v>0.23414927768860352</v>
       </c>
     </row>
@@ -1609,10 +1602,10 @@
         <v>39</v>
       </c>
       <c r="B32">
-        <v>0</v>
+        <v>14.8</v>
       </c>
       <c r="C32">
-        <v>0</v>
+        <v>11.924799999999999</v>
       </c>
       <c r="D32" s="1">
         <v>100</v>
@@ -1621,19 +1614,20 @@
         <v>4.33</v>
       </c>
       <c r="F32" s="1">
-        <v>0</v>
+        <v>78.92</v>
       </c>
       <c r="G32" s="1">
-        <v>0</v>
+        <v>9.6</v>
       </c>
       <c r="H32" s="1">
-        <v>0</v>
+        <v>47.29</v>
       </c>
       <c r="I32" s="1">
-        <v>0</v>
+        <v>43.11</v>
       </c>
       <c r="J32">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.20300274899555931</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.35">
@@ -1641,10 +1635,10 @@
         <v>40</v>
       </c>
       <c r="B33">
-        <v>14.8</v>
+        <v>15.4511</v>
       </c>
       <c r="C33">
-        <v>11.924799999999999</v>
+        <v>19.272300000000001</v>
       </c>
       <c r="D33" s="1">
         <v>100</v>
@@ -1653,20 +1647,20 @@
         <v>4.33</v>
       </c>
       <c r="F33" s="1">
-        <v>78.92</v>
+        <v>86.83</v>
       </c>
       <c r="G33" s="1">
-        <v>9.6</v>
+        <v>10.73</v>
       </c>
       <c r="H33" s="1">
-        <v>47.29</v>
+        <v>46.73</v>
       </c>
       <c r="I33" s="1">
-        <v>43.11</v>
+        <v>42.54</v>
       </c>
       <c r="J33">
         <f t="shared" si="0"/>
-        <v>0.20300274899555931</v>
+        <v>0.22961694842713462</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.35">
@@ -1674,10 +1668,10 @@
         <v>41</v>
       </c>
       <c r="B34">
-        <v>15.4511</v>
+        <v>14.8398</v>
       </c>
       <c r="C34">
-        <v>19.272300000000001</v>
+        <v>26.62</v>
       </c>
       <c r="D34" s="1">
         <v>100</v>
@@ -1686,20 +1680,20 @@
         <v>4.33</v>
       </c>
       <c r="F34" s="1">
-        <v>86.83</v>
+        <v>96.61</v>
       </c>
       <c r="G34" s="1">
-        <v>10.73</v>
+        <v>10.7</v>
       </c>
       <c r="H34" s="1">
-        <v>46.73</v>
+        <v>47.34</v>
       </c>
       <c r="I34" s="1">
-        <v>42.54</v>
+        <v>41.96</v>
       </c>
       <c r="J34">
         <f t="shared" si="0"/>
-        <v>0.22961694842713462</v>
+        <v>0.22602450359104348</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.35">
@@ -1707,10 +1701,10 @@
         <v>42</v>
       </c>
       <c r="B35">
-        <v>14.8398</v>
+        <v>14.8857</v>
       </c>
       <c r="C35">
-        <v>26.62</v>
+        <v>33.967500000000001</v>
       </c>
       <c r="D35" s="1">
         <v>100</v>
@@ -1719,20 +1713,20 @@
         <v>4.33</v>
       </c>
       <c r="F35" s="1">
-        <v>96.61</v>
+        <v>99.2</v>
       </c>
       <c r="G35" s="1">
-        <v>10.7</v>
+        <v>9.57</v>
       </c>
       <c r="H35" s="1">
-        <v>47.34</v>
+        <v>46.48</v>
       </c>
       <c r="I35" s="1">
-        <v>41.96</v>
+        <v>43.95</v>
       </c>
       <c r="J35">
         <f t="shared" si="0"/>
-        <v>0.22602450359104348</v>
+        <v>0.205895008605852</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.35">
@@ -1740,10 +1734,10 @@
         <v>43</v>
       </c>
       <c r="B36">
-        <v>14.8857</v>
+        <v>14.931699999999999</v>
       </c>
       <c r="C36">
-        <v>33.967500000000001</v>
+        <v>41.315300000000001</v>
       </c>
       <c r="D36" s="1">
         <v>100</v>
@@ -1752,20 +1746,20 @@
         <v>4.33</v>
       </c>
       <c r="F36" s="1">
-        <v>99.2</v>
+        <v>103.77</v>
       </c>
       <c r="G36" s="1">
-        <v>9.57</v>
+        <v>8.93</v>
       </c>
       <c r="H36" s="1">
-        <v>46.48</v>
+        <v>45.94</v>
       </c>
       <c r="I36" s="1">
-        <v>43.95</v>
+        <v>45.14</v>
       </c>
       <c r="J36">
         <f t="shared" si="0"/>
-        <v>0.205895008605852</v>
+        <v>0.19438397910317806</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.35">
@@ -1773,10 +1767,10 @@
         <v>44</v>
       </c>
       <c r="B37">
-        <v>14.931699999999999</v>
+        <v>25.4358</v>
       </c>
       <c r="C37">
-        <v>41.315300000000001</v>
+        <v>11.857799999999999</v>
       </c>
       <c r="D37" s="1">
         <v>100</v>
@@ -1785,20 +1779,20 @@
         <v>4.33</v>
       </c>
       <c r="F37" s="1">
-        <v>103.77</v>
+        <v>87.17</v>
       </c>
       <c r="G37" s="1">
-        <v>8.93</v>
+        <v>10.42</v>
       </c>
       <c r="H37" s="1">
-        <v>45.94</v>
+        <v>47.22</v>
       </c>
       <c r="I37" s="1">
-        <v>45.14</v>
+        <v>42.36</v>
       </c>
       <c r="J37">
         <f t="shared" si="0"/>
-        <v>0.19438397910317806</v>
+        <v>0.22066920796272765</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.35">
@@ -1806,10 +1800,10 @@
         <v>45</v>
       </c>
       <c r="B38">
-        <v>25.4358</v>
+        <v>25.4816</v>
       </c>
       <c r="C38">
-        <v>11.857799999999999</v>
+        <v>19.2056</v>
       </c>
       <c r="D38" s="1">
         <v>100</v>
@@ -1818,20 +1812,20 @@
         <v>4.33</v>
       </c>
       <c r="F38" s="1">
-        <v>87.17</v>
+        <v>95.04</v>
       </c>
       <c r="G38" s="1">
-        <v>10.42</v>
+        <v>9</v>
       </c>
       <c r="H38" s="1">
-        <v>47.22</v>
+        <v>46.41</v>
       </c>
       <c r="I38" s="1">
-        <v>42.36</v>
+        <v>44.59</v>
       </c>
       <c r="J38">
         <f t="shared" si="0"/>
-        <v>0.22066920796272765</v>
+        <v>0.19392372333548805</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.35">
@@ -1839,10 +1833,10 @@
         <v>46</v>
       </c>
       <c r="B39">
-        <v>25.4816</v>
+        <v>25.5274</v>
       </c>
       <c r="C39">
-        <v>19.2056</v>
+        <v>26.5534</v>
       </c>
       <c r="D39" s="1">
         <v>100</v>
@@ -1851,20 +1845,20 @@
         <v>4.33</v>
       </c>
       <c r="F39" s="1">
-        <v>95.04</v>
+        <v>106.85</v>
       </c>
       <c r="G39" s="1">
-        <v>9</v>
+        <v>9.7200000000000006</v>
       </c>
       <c r="H39" s="1">
-        <v>46.41</v>
+        <v>46.26</v>
       </c>
       <c r="I39" s="1">
-        <v>44.59</v>
+        <v>44.02</v>
       </c>
       <c r="J39">
         <f t="shared" si="0"/>
-        <v>0.19392372333548805</v>
+        <v>0.21011673151750976</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.35">
@@ -1872,10 +1866,10 @@
         <v>47</v>
       </c>
       <c r="B40">
-        <v>25.5274</v>
+        <v>25.5732</v>
       </c>
       <c r="C40">
-        <v>26.5534</v>
+        <v>33.900999999999996</v>
       </c>
       <c r="D40" s="1">
         <v>100</v>
@@ -1884,20 +1878,20 @@
         <v>4.33</v>
       </c>
       <c r="F40" s="1">
-        <v>106.85</v>
+        <v>110.38</v>
       </c>
       <c r="G40" s="1">
-        <v>9.7200000000000006</v>
+        <v>8.41</v>
       </c>
       <c r="H40" s="1">
-        <v>46.26</v>
+        <v>44.27</v>
       </c>
       <c r="I40" s="1">
-        <v>44.02</v>
+        <v>47.32</v>
       </c>
       <c r="J40">
         <f t="shared" si="0"/>
-        <v>0.21011673151750976</v>
+        <v>0.18997063474135983</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.35">
@@ -1905,10 +1899,10 @@
         <v>48</v>
       </c>
       <c r="B41">
-        <v>25.5732</v>
+        <v>25.6189</v>
       </c>
       <c r="C41">
-        <v>33.900999999999996</v>
+        <v>41.248800000000003</v>
       </c>
       <c r="D41" s="1">
         <v>100</v>
@@ -1917,20 +1911,20 @@
         <v>4.33</v>
       </c>
       <c r="F41" s="1">
-        <v>110.38</v>
+        <v>142.51</v>
       </c>
       <c r="G41" s="1">
-        <v>8.41</v>
+        <v>10.37</v>
       </c>
       <c r="H41" s="1">
-        <v>44.27</v>
+        <v>46.7</v>
       </c>
       <c r="I41" s="1">
-        <v>47.32</v>
+        <v>42.93</v>
       </c>
       <c r="J41">
         <f t="shared" si="0"/>
-        <v>0.18997063474135983</v>
+        <v>0.22205567451820127</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.35">
@@ -1938,10 +1932,10 @@
         <v>49</v>
       </c>
       <c r="B42">
-        <v>25.6189</v>
+        <v>36.1233</v>
       </c>
       <c r="C42">
-        <v>41.248800000000003</v>
+        <v>11.7913</v>
       </c>
       <c r="D42" s="1">
         <v>100</v>
@@ -1950,20 +1944,20 @@
         <v>4.33</v>
       </c>
       <c r="F42" s="1">
-        <v>142.51</v>
+        <v>95.73</v>
       </c>
       <c r="G42" s="1">
-        <v>10.37</v>
+        <v>9.2899999999999991</v>
       </c>
       <c r="H42" s="1">
-        <v>46.7</v>
+        <v>46.16</v>
       </c>
       <c r="I42" s="1">
-        <v>42.93</v>
+        <v>44.54</v>
       </c>
       <c r="J42">
         <f t="shared" si="0"/>
-        <v>0.22205567451820127</v>
+        <v>0.20125649913344887</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.35">
@@ -1971,10 +1965,10 @@
         <v>50</v>
       </c>
       <c r="B43">
-        <v>36.1233</v>
+        <v>36.1691</v>
       </c>
       <c r="C43">
-        <v>11.7913</v>
+        <v>19.139099999999999</v>
       </c>
       <c r="D43" s="1">
         <v>100</v>
@@ -1983,20 +1977,20 @@
         <v>4.33</v>
       </c>
       <c r="F43" s="1">
-        <v>95.73</v>
+        <v>101.87</v>
       </c>
       <c r="G43" s="1">
-        <v>9.2899999999999991</v>
+        <v>8.57</v>
       </c>
       <c r="H43" s="1">
-        <v>46.16</v>
+        <v>44.83</v>
       </c>
       <c r="I43" s="1">
-        <v>44.54</v>
+        <v>46.6</v>
       </c>
       <c r="J43">
         <f t="shared" si="0"/>
-        <v>0.20125649913344887</v>
+        <v>0.19116662948918137</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.35">
@@ -2004,10 +1998,10 @@
         <v>51</v>
       </c>
       <c r="B44">
-        <v>36.1691</v>
+        <v>36.214799999999997</v>
       </c>
       <c r="C44">
-        <v>19.139099999999999</v>
+        <v>26.486699999999999</v>
       </c>
       <c r="D44" s="1">
         <v>100</v>
@@ -2016,20 +2010,20 @@
         <v>4.33</v>
       </c>
       <c r="F44" s="1">
-        <v>101.87</v>
+        <v>114.87</v>
       </c>
       <c r="G44" s="1">
-        <v>8.57</v>
+        <v>8.2100000000000009</v>
       </c>
       <c r="H44" s="1">
-        <v>44.83</v>
+        <v>44.18</v>
       </c>
       <c r="I44" s="1">
-        <v>46.6</v>
+        <v>47.61</v>
       </c>
       <c r="J44">
         <f t="shared" si="0"/>
-        <v>0.19116662948918137</v>
+        <v>0.18583069262109553</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.35">
@@ -2037,10 +2031,10 @@
         <v>52</v>
       </c>
       <c r="B45">
-        <v>36.214799999999997</v>
+        <v>36.260800000000003</v>
       </c>
       <c r="C45">
-        <v>26.486699999999999</v>
+        <v>33.834499999999998</v>
       </c>
       <c r="D45" s="1">
         <v>100</v>
@@ -2049,20 +2043,20 @@
         <v>4.33</v>
       </c>
       <c r="F45" s="1">
-        <v>114.87</v>
+        <v>124.99</v>
       </c>
       <c r="G45" s="1">
-        <v>8.2100000000000009</v>
+        <v>8.32</v>
       </c>
       <c r="H45" s="1">
-        <v>44.18</v>
+        <v>44</v>
       </c>
       <c r="I45" s="1">
-        <v>47.61</v>
+        <v>47.67</v>
       </c>
       <c r="J45">
         <f t="shared" si="0"/>
-        <v>0.18583069262109553</v>
+        <v>0.18909090909090909</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.35">
@@ -2070,10 +2064,10 @@
         <v>53</v>
       </c>
       <c r="B46">
-        <v>36.260800000000003</v>
+        <v>36.3063</v>
       </c>
       <c r="C46">
-        <v>33.834499999999998</v>
+        <v>41.182000000000002</v>
       </c>
       <c r="D46" s="1">
         <v>100</v>
@@ -2082,20 +2076,20 @@
         <v>4.33</v>
       </c>
       <c r="F46" s="1">
-        <v>124.99</v>
+        <v>137.57</v>
       </c>
       <c r="G46" s="1">
-        <v>8.32</v>
+        <v>8.7200000000000006</v>
       </c>
       <c r="H46" s="1">
-        <v>44</v>
+        <v>43.24</v>
       </c>
       <c r="I46" s="1">
-        <v>47.67</v>
+        <v>48.04</v>
       </c>
       <c r="J46">
         <f t="shared" si="0"/>
-        <v>0.18909090909090909</v>
+        <v>0.20166512488436633</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.35">
@@ -2103,10 +2097,10 @@
         <v>54</v>
       </c>
       <c r="B47">
-        <v>36.3063</v>
+        <v>-36.386299999999999</v>
       </c>
       <c r="C47">
-        <v>41.182000000000002</v>
+        <v>8.7929999999999993</v>
       </c>
       <c r="D47" s="1">
         <v>100</v>
@@ -2115,20 +2109,20 @@
         <v>4.33</v>
       </c>
       <c r="F47" s="1">
-        <v>137.57</v>
+        <v>51.75</v>
       </c>
       <c r="G47" s="1">
-        <v>8.7200000000000006</v>
+        <v>11.95</v>
       </c>
       <c r="H47" s="1">
-        <v>43.24</v>
+        <v>50.11</v>
       </c>
       <c r="I47" s="1">
-        <v>48.04</v>
+        <v>37.93</v>
       </c>
       <c r="J47">
         <f t="shared" si="0"/>
-        <v>0.20166512488436633</v>
+        <v>0.23847535422071442</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.35">
@@ -2136,10 +2130,10 @@
         <v>55</v>
       </c>
       <c r="B48">
-        <v>-36.386299999999999</v>
+        <v>-36.340299999999999</v>
       </c>
       <c r="C48">
-        <v>8.7929999999999993</v>
+        <v>16.140599999999999</v>
       </c>
       <c r="D48" s="1">
         <v>100</v>
@@ -2148,20 +2142,20 @@
         <v>4.33</v>
       </c>
       <c r="F48" s="1">
-        <v>51.75</v>
+        <v>56.28</v>
       </c>
       <c r="G48" s="1">
-        <v>11.95</v>
+        <v>12.28</v>
       </c>
       <c r="H48" s="1">
-        <v>50.11</v>
+        <v>49.9</v>
       </c>
       <c r="I48" s="1">
-        <v>37.93</v>
+        <v>37.82</v>
       </c>
       <c r="J48">
         <f t="shared" si="0"/>
-        <v>0.23847535422071442</v>
+        <v>0.24609218436873748</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.35">
@@ -2169,10 +2163,10 @@
         <v>56</v>
       </c>
       <c r="B49">
-        <v>-36.340299999999999</v>
+        <v>-36.2943</v>
       </c>
       <c r="C49">
-        <v>16.140599999999999</v>
+        <v>23.488299999999999</v>
       </c>
       <c r="D49" s="1">
         <v>100</v>
@@ -2181,20 +2175,20 @@
         <v>4.33</v>
       </c>
       <c r="F49" s="1">
-        <v>56.28</v>
+        <v>58.38</v>
       </c>
       <c r="G49" s="1">
-        <v>12.28</v>
+        <v>11.86</v>
       </c>
       <c r="H49" s="1">
-        <v>49.9</v>
+        <v>49.4</v>
       </c>
       <c r="I49" s="1">
-        <v>37.82</v>
+        <v>38.75</v>
       </c>
       <c r="J49">
         <f t="shared" si="0"/>
-        <v>0.24609218436873748</v>
+        <v>0.24008097165991901</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.35">
@@ -2202,10 +2196,10 @@
         <v>57</v>
       </c>
       <c r="B50">
-        <v>-36.2943</v>
+        <v>-36.249099999999999</v>
       </c>
       <c r="C50">
-        <v>23.488299999999999</v>
+        <v>30.836100000000002</v>
       </c>
       <c r="D50" s="1">
         <v>100</v>
@@ -2214,20 +2208,20 @@
         <v>4.33</v>
       </c>
       <c r="F50" s="1">
-        <v>58.38</v>
+        <v>59.93</v>
       </c>
       <c r="G50" s="1">
-        <v>11.86</v>
+        <v>11.4</v>
       </c>
       <c r="H50" s="1">
-        <v>49.4</v>
+        <v>49.82</v>
       </c>
       <c r="I50" s="1">
-        <v>38.75</v>
+        <v>38.78</v>
       </c>
       <c r="J50">
         <f t="shared" si="0"/>
-        <v>0.24008097165991901</v>
+        <v>0.22882376555600162</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.35">
@@ -2235,10 +2229,10 @@
         <v>58</v>
       </c>
       <c r="B51">
-        <v>-36.249099999999999</v>
+        <v>-36.203099999999999</v>
       </c>
       <c r="C51">
-        <v>30.836100000000002</v>
+        <v>38.183799999999998</v>
       </c>
       <c r="D51" s="1">
         <v>100</v>
@@ -2247,20 +2241,20 @@
         <v>4.33</v>
       </c>
       <c r="F51" s="1">
-        <v>59.93</v>
+        <v>65.38</v>
       </c>
       <c r="G51" s="1">
-        <v>11.4</v>
+        <v>11.74</v>
       </c>
       <c r="H51" s="1">
-        <v>49.82</v>
+        <v>49.83</v>
       </c>
       <c r="I51" s="1">
-        <v>38.78</v>
+        <v>38.43</v>
       </c>
       <c r="J51">
         <f t="shared" si="0"/>
-        <v>0.22882376555600162</v>
+        <v>0.23560104354806344</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.35">
@@ -2268,10 +2262,10 @@
         <v>59</v>
       </c>
       <c r="B52">
-        <v>-36.203099999999999</v>
+        <v>-25.698799999999999</v>
       </c>
       <c r="C52">
-        <v>38.183799999999998</v>
+        <v>8.7262999999999984</v>
       </c>
       <c r="D52" s="1">
         <v>100</v>
@@ -2280,20 +2274,20 @@
         <v>4.33</v>
       </c>
       <c r="F52" s="1">
-        <v>65.38</v>
+        <v>63.91</v>
       </c>
       <c r="G52" s="1">
-        <v>11.74</v>
+        <v>11.9</v>
       </c>
       <c r="H52" s="1">
-        <v>49.83</v>
+        <v>49.63</v>
       </c>
       <c r="I52" s="1">
-        <v>38.43</v>
+        <v>38.47</v>
       </c>
       <c r="J52">
         <f t="shared" si="0"/>
-        <v>0.23560104354806344</v>
+        <v>0.23977433004231311</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.35">
@@ -2301,10 +2295,10 @@
         <v>60</v>
       </c>
       <c r="B53">
-        <v>-25.698799999999999</v>
+        <v>-25.652899999999999</v>
       </c>
       <c r="C53">
-        <v>8.7262999999999984</v>
+        <v>16.073999999999998</v>
       </c>
       <c r="D53" s="1">
         <v>100</v>
@@ -2313,20 +2307,20 @@
         <v>4.33</v>
       </c>
       <c r="F53" s="1">
-        <v>63.91</v>
+        <v>64.83</v>
       </c>
       <c r="G53" s="1">
-        <v>11.9</v>
+        <v>11.62</v>
       </c>
       <c r="H53" s="1">
-        <v>49.63</v>
+        <v>49.26</v>
       </c>
       <c r="I53" s="1">
-        <v>38.47</v>
+        <v>39.119999999999997</v>
       </c>
       <c r="J53">
         <f t="shared" si="0"/>
-        <v>0.23977433004231311</v>
+        <v>0.23589118960617134</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.35">
@@ -2334,10 +2328,10 @@
         <v>61</v>
       </c>
       <c r="B54">
-        <v>-25.652899999999999</v>
+        <v>-25.607099999999999</v>
       </c>
       <c r="C54">
-        <v>16.073999999999998</v>
+        <v>23.4221</v>
       </c>
       <c r="D54" s="1">
         <v>100</v>
@@ -2346,20 +2340,20 @@
         <v>4.33</v>
       </c>
       <c r="F54" s="1">
-        <v>64.83</v>
+        <v>68.989999999999995</v>
       </c>
       <c r="G54" s="1">
-        <v>11.62</v>
+        <v>12.17</v>
       </c>
       <c r="H54" s="1">
-        <v>49.26</v>
+        <v>50.43</v>
       </c>
       <c r="I54" s="1">
-        <v>39.119999999999997</v>
+        <v>37.4</v>
       </c>
       <c r="J54">
         <f t="shared" si="0"/>
-        <v>0.23589118960617134</v>
+        <v>0.2413246083680349</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.35">
@@ -2367,10 +2361,10 @@
         <v>62</v>
       </c>
       <c r="B55">
-        <v>-25.607099999999999</v>
+        <v>-25.561199999999999</v>
       </c>
       <c r="C55">
-        <v>23.4221</v>
+        <v>30.7699</v>
       </c>
       <c r="D55" s="1">
         <v>100</v>
@@ -2379,20 +2373,20 @@
         <v>4.33</v>
       </c>
       <c r="F55" s="1">
-        <v>68.989999999999995</v>
+        <v>74.14</v>
       </c>
       <c r="G55" s="1">
-        <v>12.17</v>
+        <v>10.96</v>
       </c>
       <c r="H55" s="1">
-        <v>50.43</v>
+        <v>48.26</v>
       </c>
       <c r="I55" s="1">
-        <v>37.4</v>
+        <v>40.78</v>
       </c>
       <c r="J55">
         <f t="shared" si="0"/>
-        <v>0.2413246083680349</v>
+        <v>0.22710319104848739</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.35">
@@ -2400,10 +2394,10 @@
         <v>63</v>
       </c>
       <c r="B56">
-        <v>-25.561199999999999</v>
+        <v>-25.515699999999999</v>
       </c>
       <c r="C56">
-        <v>30.7699</v>
+        <v>38.1173</v>
       </c>
       <c r="D56" s="1">
         <v>100</v>
@@ -2412,20 +2406,20 @@
         <v>4.33</v>
       </c>
       <c r="F56" s="1">
-        <v>74.14</v>
+        <v>75.92</v>
       </c>
       <c r="G56" s="1">
-        <v>10.96</v>
+        <v>11.65</v>
       </c>
       <c r="H56" s="1">
-        <v>48.26</v>
+        <v>48.5</v>
       </c>
       <c r="I56" s="1">
-        <v>40.78</v>
+        <v>39.85</v>
       </c>
       <c r="J56">
         <f t="shared" si="0"/>
-        <v>0.22710319104848739</v>
+        <v>0.24020618556701032</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.35">
@@ -2433,10 +2427,10 @@
         <v>64</v>
       </c>
       <c r="B57">
-        <v>-25.515699999999999</v>
+        <v>-15.011200000000001</v>
       </c>
       <c r="C57">
-        <v>38.1173</v>
+        <v>8.6597000000000008</v>
       </c>
       <c r="D57" s="1">
         <v>100</v>
@@ -2445,20 +2439,20 @@
         <v>4.33</v>
       </c>
       <c r="F57" s="1">
-        <v>75.92</v>
+        <v>61.15</v>
       </c>
       <c r="G57" s="1">
-        <v>11.65</v>
+        <v>8.14</v>
       </c>
       <c r="H57" s="1">
-        <v>48.5</v>
+        <v>46.29</v>
       </c>
       <c r="I57" s="1">
-        <v>39.85</v>
+        <v>45.57</v>
       </c>
       <c r="J57">
         <f t="shared" si="0"/>
-        <v>0.24020618556701032</v>
+        <v>0.17584791531648306</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.35">
@@ -2466,10 +2460,10 @@
         <v>65</v>
       </c>
       <c r="B58">
-        <v>-15.011200000000001</v>
+        <v>-14.965199999999999</v>
       </c>
       <c r="C58">
-        <v>8.6597000000000008</v>
+        <v>16.0075</v>
       </c>
       <c r="D58" s="1">
         <v>100</v>
@@ -2478,20 +2472,20 @@
         <v>4.33</v>
       </c>
       <c r="F58" s="1">
-        <v>61.15</v>
+        <v>74.930000000000007</v>
       </c>
       <c r="G58" s="1">
-        <v>8.14</v>
+        <v>10.16</v>
       </c>
       <c r="H58" s="1">
-        <v>46.29</v>
+        <v>47.56</v>
       </c>
       <c r="I58" s="1">
-        <v>45.57</v>
+        <v>42.28</v>
       </c>
       <c r="J58">
         <f t="shared" si="0"/>
-        <v>0.17584791531648306</v>
+        <v>0.21362489486963834</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.35">
@@ -2499,10 +2493,10 @@
         <v>66</v>
       </c>
       <c r="B59">
-        <v>-14.965199999999999</v>
+        <v>-14.9194</v>
       </c>
       <c r="C59">
-        <v>16.0075</v>
+        <v>23.3553</v>
       </c>
       <c r="D59" s="1">
         <v>100</v>
@@ -2511,20 +2505,20 @@
         <v>4.33</v>
       </c>
       <c r="F59" s="1">
-        <v>74.930000000000007</v>
+        <v>76.45</v>
       </c>
       <c r="G59" s="1">
-        <v>10.16</v>
+        <v>10.15</v>
       </c>
       <c r="H59" s="1">
-        <v>47.56</v>
+        <v>48.31</v>
       </c>
       <c r="I59" s="1">
-        <v>42.28</v>
+        <v>41.54</v>
       </c>
       <c r="J59">
         <f t="shared" si="0"/>
-        <v>0.21362489486963834</v>
+        <v>0.21010142827571932</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.35">
@@ -2532,10 +2526,10 @@
         <v>67</v>
       </c>
       <c r="B60">
-        <v>-14.9194</v>
+        <v>-14.873900000000001</v>
       </c>
       <c r="C60">
-        <v>23.3553</v>
+        <v>30.7028</v>
       </c>
       <c r="D60" s="1">
         <v>100</v>
@@ -2544,20 +2538,20 @@
         <v>4.33</v>
       </c>
       <c r="F60" s="1">
-        <v>76.45</v>
+        <v>81.87</v>
       </c>
       <c r="G60" s="1">
-        <v>10.15</v>
+        <v>10.49</v>
       </c>
       <c r="H60" s="1">
-        <v>48.31</v>
+        <v>47.26</v>
       </c>
       <c r="I60" s="1">
-        <v>41.54</v>
+        <v>42.25</v>
       </c>
       <c r="J60">
         <f t="shared" si="0"/>
-        <v>0.21010142827571932</v>
+        <v>0.22196360558611936</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.35">
@@ -2565,10 +2559,10 @@
         <v>68</v>
       </c>
       <c r="B61">
-        <v>-14.873900000000001</v>
+        <v>-14.828099999999999</v>
       </c>
       <c r="C61">
-        <v>30.7028</v>
+        <v>38.0505</v>
       </c>
       <c r="D61" s="1">
         <v>100</v>
@@ -2577,51 +2571,18 @@
         <v>4.33</v>
       </c>
       <c r="F61" s="1">
-        <v>81.87</v>
+        <v>86.18</v>
       </c>
       <c r="G61" s="1">
-        <v>10.49</v>
+        <v>9.6199999999999992</v>
       </c>
       <c r="H61" s="1">
         <v>47.26</v>
       </c>
       <c r="I61" s="1">
-        <v>42.25</v>
+        <v>43.12</v>
       </c>
       <c r="J61">
-        <f t="shared" si="0"/>
-        <v>0.22196360558611936</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A62" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B62">
-        <v>-14.828099999999999</v>
-      </c>
-      <c r="C62">
-        <v>38.0505</v>
-      </c>
-      <c r="D62" s="1">
-        <v>100</v>
-      </c>
-      <c r="E62" s="1">
-        <v>4.33</v>
-      </c>
-      <c r="F62" s="1">
-        <v>86.18</v>
-      </c>
-      <c r="G62" s="1">
-        <v>9.6199999999999992</v>
-      </c>
-      <c r="H62" s="1">
-        <v>47.26</v>
-      </c>
-      <c r="I62" s="1">
-        <v>43.12</v>
-      </c>
-      <c r="J62">
         <f t="shared" si="0"/>
         <v>0.20355480321625052</v>
       </c>

</xml_diff>